<commit_message>
Deploying to gh-pages from  @ 8afc4bd5e0dbda61763062e5721505f52a5c15ab 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-3-2.xlsx
+++ b/assets/excel/2021_1-3-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C913348D-ABDF-441E-A8A8-22DA33A4AB36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA977A-BB3D-4ED8-91DD-34831BBA74F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{D818978F-F71E-4D9C-8ED8-548A62D97831}"/>
   </bookViews>
@@ -538,6 +538,9 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -594,9 +597,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -916,8 +916,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:M172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A157" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,61 +954,61 @@
       <c r="G4" s="1"/>
     </row>
     <row r="6" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
     </row>
     <row r="7" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="48" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="51" t="s">
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="51" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="51" t="s">
+      <c r="H8" s="53"/>
+      <c r="I8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="53"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1020,9 +1020,9 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="47"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="6">
         <v>1000</v>
       </c>
@@ -1041,11 +1041,11 @@
       <c r="J9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="54">
+      <c r="K9" s="55">
         <v>1000</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="56"/>
     </row>
     <row r="10" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
@@ -1702,13 +1702,13 @@
         <v>34.417408007946591</v>
       </c>
       <c r="K27" s="11">
-        <v>735.98018999999999</v>
+        <v>103.07277000000001</v>
       </c>
       <c r="L27" s="11">
-        <v>103.07277000000001</v>
+        <v>44.397529999999996</v>
       </c>
       <c r="M27" s="11">
-        <v>44.397529999999996</v>
+        <v>93.498339999999999</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1738,13 +1738,13 @@
         <v>32.416105097216942</v>
       </c>
       <c r="K28" s="11">
-        <v>479.79467999999997</v>
+        <v>42.428899999999999</v>
       </c>
       <c r="L28" s="11">
-        <v>42.428899999999999</v>
+        <v>19.416730000000001</v>
       </c>
       <c r="M28" s="11">
-        <v>19.416730000000001</v>
+        <v>42.408319999999996</v>
       </c>
     </row>
     <row r="29" spans="2:13" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1776,13 +1776,13 @@
         <v>33.81303349818446</v>
       </c>
       <c r="K29" s="17">
-        <v>1215.7748700000002</v>
+        <v>145.50167000000002</v>
       </c>
       <c r="L29" s="17">
-        <v>145.50167000000002</v>
+        <v>63.814260000000004</v>
       </c>
       <c r="M29" s="17">
-        <v>63.814260000000004</v>
+        <v>135.90667000000002</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1814,13 +1814,13 @@
         <v>35.283233219214864</v>
       </c>
       <c r="K30" s="11">
-        <v>784.15094999999997</v>
+        <v>159.72075000000001</v>
       </c>
       <c r="L30" s="11">
-        <v>159.72075000000001</v>
+        <v>39.890329999999999</v>
       </c>
       <c r="M30" s="11">
-        <v>39.890329999999999</v>
+        <v>147.85239999999999</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1852,13 +1852,13 @@
         <v>34.7946217302161</v>
       </c>
       <c r="K31" s="11">
-        <v>325.80624</v>
+        <v>91.846050000000005</v>
       </c>
       <c r="L31" s="11">
-        <v>91.846050000000005</v>
+        <v>20.654400000000003</v>
       </c>
       <c r="M31" s="11">
-        <v>20.654400000000003</v>
+        <v>89.197130000000001</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>35.959329308157812</v>
       </c>
       <c r="K32" s="11">
-        <v>458.34471000000002</v>
+        <v>67.87469999999999</v>
       </c>
       <c r="L32" s="11">
-        <v>67.87469999999999</v>
+        <v>19.23593</v>
       </c>
       <c r="M32" s="11">
-        <v>19.23593</v>
+        <v>58.655269999999994</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1926,13 +1926,13 @@
         <v>30.808510692606621</v>
       </c>
       <c r="K33" s="11">
-        <v>375.69541999999996</v>
+        <v>43.481569999999998</v>
       </c>
       <c r="L33" s="11">
-        <v>43.481569999999998</v>
+        <v>22.718240000000002</v>
       </c>
       <c r="M33" s="11">
-        <v>22.718240000000002</v>
+        <v>43.496079999999999</v>
       </c>
     </row>
     <row r="34" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>35.679913719592072</v>
       </c>
       <c r="K34" s="11">
-        <v>395.22775000000001</v>
+        <v>38.967309999999998</v>
       </c>
       <c r="L34" s="11">
-        <v>38.967309999999998</v>
+        <v>14.056089999999999</v>
       </c>
       <c r="M34" s="11">
-        <v>14.056089999999999</v>
+        <v>35.339649999999999</v>
       </c>
     </row>
     <row r="35" spans="2:13" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2000,13 +2000,13 @@
         <v>34.447691444102333</v>
       </c>
       <c r="K35" s="17">
-        <v>1555.0741200000002</v>
+        <v>242.16964000000002</v>
       </c>
       <c r="L35" s="17">
-        <v>242.16964000000002</v>
+        <v>76.664649999999995</v>
       </c>
       <c r="M35" s="17">
-        <v>76.664649999999995</v>
+        <v>226.68813</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,13 +2036,13 @@
         <v>36.793428097985114</v>
       </c>
       <c r="K36" s="11">
-        <v>752.57431000000008</v>
+        <v>65.021280000000004</v>
       </c>
       <c r="L36" s="11">
-        <v>65.021280000000004</v>
+        <v>19.552619999999997</v>
       </c>
       <c r="M36" s="11">
-        <v>19.552619999999997</v>
+        <v>77.539289999999994</v>
       </c>
     </row>
     <row r="37" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2072,13 +2072,13 @@
         <v>34.265912836032022</v>
       </c>
       <c r="K37" s="11">
-        <v>624.19130000000007</v>
+        <v>56.90699</v>
       </c>
       <c r="L37" s="11">
-        <v>56.90699</v>
+        <v>18.322279999999999</v>
       </c>
       <c r="M37" s="11">
-        <v>18.322279999999999</v>
+        <v>57.331009999999999</v>
       </c>
     </row>
     <row r="38" spans="2:13" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2110,13 +2110,13 @@
         <v>35.656414391713454</v>
       </c>
       <c r="K38" s="17">
-        <v>1376.7656100000002</v>
+        <v>121.92827</v>
       </c>
       <c r="L38" s="17">
-        <v>121.92827</v>
+        <v>37.874900000000004</v>
       </c>
       <c r="M38" s="17">
-        <v>37.874900000000004</v>
+        <v>134.87029999999999</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2146,13 +2146,13 @@
         <v>33.187116706127931</v>
       </c>
       <c r="K39" s="11">
-        <v>608.61858999999993</v>
+        <v>54.569319999999998</v>
       </c>
       <c r="L39" s="11">
-        <v>54.569319999999998</v>
+        <v>15.27867</v>
       </c>
       <c r="M39" s="11">
-        <v>15.27867</v>
+        <v>44.010460000000002</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2182,13 +2182,13 @@
         <v>33.888031876867693</v>
       </c>
       <c r="K40" s="11">
-        <v>521.65695000000005</v>
+        <v>51.998440000000002</v>
       </c>
       <c r="L40" s="11">
-        <v>51.998440000000002</v>
+        <v>30.461880000000001</v>
       </c>
       <c r="M40" s="11">
-        <v>30.461880000000001</v>
+        <v>58.261160000000004</v>
       </c>
     </row>
     <row r="41" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2218,13 +2218,13 @@
         <v>29.733428010841216</v>
       </c>
       <c r="K41" s="11">
-        <v>819.52831999999989</v>
+        <v>134.04888</v>
       </c>
       <c r="L41" s="11">
-        <v>134.04888</v>
+        <v>58.97766</v>
       </c>
       <c r="M41" s="11">
-        <v>58.97766</v>
+        <v>93.08153999999999</v>
       </c>
     </row>
     <row r="42" spans="2:13" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2256,13 +2256,13 @@
         <v>31.542003307970525</v>
       </c>
       <c r="K42" s="17">
-        <v>1949.8038600000002</v>
+        <v>240.61664000000002</v>
       </c>
       <c r="L42" s="17">
-        <v>240.61664000000002</v>
+        <v>104.71821000000001</v>
       </c>
       <c r="M42" s="17">
-        <v>104.71821000000001</v>
+        <v>195.35316</v>
       </c>
     </row>
     <row r="43" spans="2:13" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2294,13 +2294,13 @@
         <v>33.616925338134848</v>
       </c>
       <c r="K43" s="17">
-        <v>6097.4184500000001</v>
+        <v>750.21622000000002</v>
       </c>
       <c r="L43" s="17">
-        <v>750.21622000000002</v>
+        <v>283.07202000000001</v>
       </c>
       <c r="M43" s="17">
-        <v>283.07202000000001</v>
+        <v>692.81825000000003</v>
       </c>
     </row>
     <row r="44" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6703,34 +6703,34 @@
       <c r="C163" s="32"/>
     </row>
     <row r="164" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C164" s="37" t="s">
+      <c r="C164" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D164" s="37"/>
-      <c r="E164" s="37"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="37"/>
-      <c r="H164" s="37"/>
-      <c r="I164" s="37"/>
-      <c r="J164" s="37"/>
-      <c r="K164" s="37"/>
-      <c r="L164" s="37"/>
-      <c r="M164" s="37"/>
+      <c r="D164" s="38"/>
+      <c r="E164" s="38"/>
+      <c r="F164" s="38"/>
+      <c r="G164" s="38"/>
+      <c r="H164" s="38"/>
+      <c r="I164" s="38"/>
+      <c r="J164" s="38"/>
+      <c r="K164" s="38"/>
+      <c r="L164" s="38"/>
+      <c r="M164" s="38"/>
     </row>
     <row r="165" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C165" s="38" t="s">
+      <c r="C165" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D165" s="38"/>
-      <c r="E165" s="38"/>
-      <c r="F165" s="38"/>
-      <c r="G165" s="38"/>
-      <c r="H165" s="38"/>
-      <c r="I165" s="38"/>
-      <c r="J165" s="38"/>
-      <c r="K165" s="38"/>
-      <c r="L165" s="38"/>
-      <c r="M165" s="38"/>
+      <c r="D165" s="39"/>
+      <c r="E165" s="39"/>
+      <c r="F165" s="39"/>
+      <c r="G165" s="39"/>
+      <c r="H165" s="39"/>
+      <c r="I165" s="39"/>
+      <c r="J165" s="39"/>
+      <c r="K165" s="39"/>
+      <c r="L165" s="39"/>
+      <c r="M165" s="39"/>
     </row>
     <row r="166" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="33"/>
@@ -6795,7 +6795,7 @@
       <c r="H171" s="34"/>
     </row>
     <row r="172" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C172" s="56" t="s">
+      <c r="C172" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D172" s="35"/>

</xml_diff>